<commit_message>
Feature import multiple audio file
</commit_message>
<xml_diff>
--- a/emotion_recognition_report.xlsx
+++ b/emotion_recognition_report.xlsx
@@ -1977,8 +1977,8 @@
   </sheetPr>
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C102" activeCellId="0" sqref="C102"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D103" activeCellId="0" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2109,6 +2109,7 @@
         <v>17</v>
       </c>
       <c r="L3" s="3" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -2303,6 +2304,7 @@
         <v>31</v>
       </c>
       <c r="L8" s="3" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -2848,6 +2850,7 @@
         <v>17</v>
       </c>
       <c r="L22" s="3" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -2886,6 +2889,7 @@
         <v>17</v>
       </c>
       <c r="L23" s="3" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -5654,6 +5658,7 @@
         <v>31</v>
       </c>
       <c r="L94" s="3" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -5692,6 +5697,7 @@
         <v>31</v>
       </c>
       <c r="L95" s="3" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>